<commit_message>
Order handling backend and frontend
</commit_message>
<xml_diff>
--- a/SQL Tables.xlsx
+++ b/SQL Tables.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Apoorv\Documents\San Jose State University\Fall 2020\CMPE 273\Assignments\Lab 1\Yelp-Prototype\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C6E195-2CE9-4E49-883F-383223C0AC4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5F86CC-C310-461F-B57E-6F67FFE5D74A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Draft" sheetId="1" r:id="rId1"/>
+    <sheet name="Tables" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$D$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Tables!$A$1:$D$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="162">
   <si>
     <t>Customer</t>
   </si>
@@ -265,15 +265,6 @@
   </si>
   <si>
     <t>Foreign key to Customer(Customer ID)</t>
-  </si>
-  <si>
-    <t>delivery</t>
-  </si>
-  <si>
-    <t>pickup</t>
-  </si>
-  <si>
-    <t>return</t>
   </si>
   <si>
     <t>Foreign key to Login(ID)</t>
@@ -655,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -671,17 +662,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -998,7 +990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -1171,10 +1163,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G142"/>
+  <dimension ref="A1:E142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A141" sqref="A141:A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1201,8 +1193,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="14" t="s">
-        <v>90</v>
+      <c r="A2" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>39</v>
@@ -1211,11 +1203,11 @@
         <v>43</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="15"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="5" t="s">
         <v>40</v>
       </c>
@@ -1225,7 +1217,7 @@
       <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="15"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="5" t="s">
         <v>41</v>
       </c>
@@ -1235,7 +1227,7 @@
       <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="15"/>
+      <c r="A5" s="13"/>
       <c r="B5" s="5" t="s">
         <v>42</v>
       </c>
@@ -1245,7 +1237,7 @@
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="15"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="5" t="s">
         <v>47</v>
       </c>
@@ -1261,23 +1253,23 @@
       <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="14" t="s">
-        <v>97</v>
+      <c r="A8" s="12" t="s">
+        <v>94</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="15"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="5" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>51</v>
@@ -1287,7 +1279,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="15"/>
+      <c r="A10" s="13"/>
       <c r="B10" s="5" t="s">
         <v>48</v>
       </c>
@@ -1297,9 +1289,9 @@
       <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="15"/>
+      <c r="A11" s="13"/>
       <c r="B11" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>44</v>
@@ -1307,7 +1299,7 @@
       <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="15"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="5" t="s">
         <v>49</v>
       </c>
@@ -1317,7 +1309,7 @@
       <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="15"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="5" t="s">
         <v>24</v>
       </c>
@@ -1327,7 +1319,7 @@
       <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="15"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
@@ -1337,9 +1329,9 @@
       <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="15"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>43</v>
@@ -1347,9 +1339,9 @@
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="15"/>
+      <c r="A16" s="13"/>
       <c r="B16" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>65</v>
@@ -1357,7 +1349,7 @@
       <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="15"/>
+      <c r="A17" s="13"/>
       <c r="B17" s="5" t="s">
         <v>54</v>
       </c>
@@ -1367,9 +1359,9 @@
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="15"/>
+      <c r="A18" s="13"/>
       <c r="B18" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>56</v>
@@ -1377,9 +1369,9 @@
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="16"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="5" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>56</v>
@@ -1393,32 +1385,32 @@
       <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="14" t="s">
-        <v>99</v>
+      <c r="A21" s="12" t="s">
+        <v>96</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>149</v>
+        <v>147</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="16"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D22" s="5"/>
-      <c r="E22" s="13"/>
+      <c r="E22" s="21"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="7"/>
@@ -1428,11 +1420,11 @@
       <c r="E23" s="10"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="11" t="s">
-        <v>154</v>
+      <c r="A24" s="20" t="s">
+        <v>151</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>51</v>
@@ -1441,12 +1433,12 @@
       <c r="E24" s="10"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A25" s="12"/>
+      <c r="A25" s="18"/>
       <c r="B25" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="10"/>
@@ -1459,22 +1451,22 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="17" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="11"/>
+      <c r="A28" s="20"/>
       <c r="B28" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>51</v>
@@ -1484,9 +1476,9 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" s="12"/>
+      <c r="A29" s="18"/>
       <c r="B29" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C29" s="5" t="s">
         <v>58</v>
@@ -1501,20 +1493,20 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="17" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="12"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="5" t="s">
         <v>47</v>
       </c>
@@ -1531,22 +1523,22 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="17" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A35" s="12"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C35" s="5" t="s">
         <v>63</v>
@@ -1560,23 +1552,23 @@
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" ht="14.1" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" s="14" t="s">
-        <v>151</v>
+      <c r="A37" s="12" t="s">
+        <v>148</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="15"/>
+      <c r="A38" s="13"/>
       <c r="B38" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>51</v>
@@ -1586,7 +1578,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" s="15"/>
+      <c r="A39" s="13"/>
       <c r="B39" s="5" t="s">
         <v>60</v>
       </c>
@@ -1596,7 +1588,7 @@
       <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="15"/>
+      <c r="A40" s="13"/>
       <c r="B40" s="5" t="s">
         <v>61</v>
       </c>
@@ -1606,9 +1598,9 @@
       <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="15"/>
+      <c r="A41" s="13"/>
       <c r="B41" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>51</v>
@@ -1618,17 +1610,17 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="15"/>
+      <c r="A42" s="13"/>
       <c r="B42" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="15"/>
+      <c r="A43" s="13"/>
       <c r="B43" s="5" t="s">
         <v>54</v>
       </c>
@@ -1638,9 +1630,9 @@
       <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="16"/>
+      <c r="A44" s="14"/>
       <c r="B44" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>65</v>
@@ -1654,23 +1646,23 @@
       <c r="D45" s="5"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="14" t="s">
-        <v>116</v>
+      <c r="A46" s="12" t="s">
+        <v>113</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A47" s="15"/>
+      <c r="A47" s="13"/>
       <c r="B47" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>51</v>
@@ -1680,7 +1672,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A48" s="15"/>
+      <c r="A48" s="13"/>
       <c r="B48" s="5" t="s">
         <v>60</v>
       </c>
@@ -1690,7 +1682,7 @@
       <c r="D48" s="5"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A49" s="15"/>
+      <c r="A49" s="13"/>
       <c r="B49" s="5" t="s">
         <v>61</v>
       </c>
@@ -1700,9 +1692,9 @@
       <c r="D49" s="5"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="15"/>
+      <c r="A50" s="13"/>
       <c r="B50" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>51</v>
@@ -1712,17 +1704,17 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A51" s="15"/>
+      <c r="A51" s="13"/>
       <c r="B51" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D51" s="5"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" s="15"/>
+      <c r="A52" s="13"/>
       <c r="B52" s="5" t="s">
         <v>54</v>
       </c>
@@ -1732,9 +1724,9 @@
       <c r="D52" s="5"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" s="16"/>
+      <c r="A53" s="14"/>
       <c r="B53" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>65</v>
@@ -1748,23 +1740,23 @@
       <c r="D54" s="5"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A55" s="14" t="s">
-        <v>117</v>
+      <c r="A55" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A56" s="15"/>
+      <c r="A56" s="13"/>
       <c r="B56" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>51</v>
@@ -1774,7 +1766,7 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A57" s="15"/>
+      <c r="A57" s="13"/>
       <c r="B57" s="5" t="s">
         <v>60</v>
       </c>
@@ -1784,7 +1776,7 @@
       <c r="D57" s="5"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A58" s="15"/>
+      <c r="A58" s="13"/>
       <c r="B58" s="5" t="s">
         <v>61</v>
       </c>
@@ -1794,9 +1786,9 @@
       <c r="D58" s="5"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" s="15"/>
+      <c r="A59" s="13"/>
       <c r="B59" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>51</v>
@@ -1806,17 +1798,17 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" s="15"/>
+      <c r="A60" s="13"/>
       <c r="B60" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D60" s="5"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A61" s="15"/>
+      <c r="A61" s="13"/>
       <c r="B61" s="5" t="s">
         <v>54</v>
       </c>
@@ -1826,9 +1818,9 @@
       <c r="D61" s="5"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" s="16"/>
+      <c r="A62" s="14"/>
       <c r="B62" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C62" s="5" t="s">
         <v>65</v>
@@ -1842,23 +1834,23 @@
       <c r="D63" s="5"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A64" s="14" t="s">
-        <v>119</v>
+      <c r="A64" s="12" t="s">
+        <v>116</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C64" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A65" s="15"/>
+      <c r="A65" s="13"/>
       <c r="B65" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>51</v>
@@ -1868,7 +1860,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A66" s="15"/>
+      <c r="A66" s="13"/>
       <c r="B66" s="5" t="s">
         <v>60</v>
       </c>
@@ -1876,11 +1868,11 @@
         <v>44</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A67" s="15"/>
+      <c r="A67" s="13"/>
       <c r="B67" s="5" t="s">
         <v>61</v>
       </c>
@@ -1890,9 +1882,9 @@
       <c r="D67" s="5"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="15"/>
+      <c r="A68" s="13"/>
       <c r="B68" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C68" s="5" t="s">
         <v>51</v>
@@ -1902,17 +1894,17 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="15"/>
+      <c r="A69" s="13"/>
       <c r="B69" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D69" s="5"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A70" s="15"/>
+      <c r="A70" s="13"/>
       <c r="B70" s="5" t="s">
         <v>54</v>
       </c>
@@ -1922,9 +1914,9 @@
       <c r="D70" s="5"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A71" s="16"/>
+      <c r="A71" s="14"/>
       <c r="B71" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C71" s="5" t="s">
         <v>65</v>
@@ -1938,23 +1930,23 @@
       <c r="D72" s="5"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A73" s="14" t="s">
-        <v>121</v>
+      <c r="A73" s="12" t="s">
+        <v>118</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C73" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A74" s="15"/>
+      <c r="A74" s="13"/>
       <c r="B74" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C74" s="5" t="s">
         <v>51</v>
@@ -1964,7 +1956,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A75" s="15"/>
+      <c r="A75" s="13"/>
       <c r="B75" s="5" t="s">
         <v>60</v>
       </c>
@@ -1974,7 +1966,7 @@
       <c r="D75" s="5"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" s="15"/>
+      <c r="A76" s="13"/>
       <c r="B76" s="5" t="s">
         <v>61</v>
       </c>
@@ -1984,9 +1976,9 @@
       <c r="D76" s="5"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A77" s="15"/>
+      <c r="A77" s="13"/>
       <c r="B77" s="5" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C77" s="5" t="s">
         <v>51</v>
@@ -1996,17 +1988,17 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A78" s="15"/>
+      <c r="A78" s="13"/>
       <c r="B78" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D78" s="5"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A79" s="15"/>
+      <c r="A79" s="13"/>
       <c r="B79" s="5" t="s">
         <v>54</v>
       </c>
@@ -2016,9 +2008,9 @@
       <c r="D79" s="5"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A80" s="16"/>
+      <c r="A80" s="14"/>
       <c r="B80" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C80" s="5" t="s">
         <v>65</v>
@@ -2032,23 +2024,23 @@
       <c r="D81" s="5"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A82" s="14" t="s">
-        <v>123</v>
+      <c r="A82" s="12" t="s">
+        <v>120</v>
       </c>
       <c r="B82" s="5" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C82" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A83" s="15"/>
+      <c r="A83" s="13"/>
       <c r="B83" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C83" s="5" t="s">
         <v>51</v>
@@ -2058,9 +2050,9 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A84" s="15"/>
+      <c r="A84" s="13"/>
       <c r="B84" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C84" s="5"/>
       <c r="D84" s="5" t="s">
@@ -2068,7 +2060,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A85" s="15"/>
+      <c r="A85" s="13"/>
       <c r="B85" s="5" t="s">
         <v>66</v>
       </c>
@@ -2080,7 +2072,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A86" s="15"/>
+      <c r="A86" s="13"/>
       <c r="B86" s="5" t="s">
         <v>52</v>
       </c>
@@ -2090,7 +2082,7 @@
       <c r="D86" s="5"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A87" s="16"/>
+      <c r="A87" s="14"/>
       <c r="B87" s="5" t="s">
         <v>67</v>
       </c>
@@ -2102,7 +2094,7 @@
     <row r="88" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="5"/>
       <c r="B88" s="5" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C88" s="5" t="s">
         <v>65</v>
@@ -2110,29 +2102,29 @@
       <c r="D88" s="5"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A89" s="21"/>
+      <c r="A89" s="11"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A90" s="14" t="s">
-        <v>126</v>
+      <c r="A90" s="12" t="s">
+        <v>123</v>
       </c>
       <c r="B90" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C90" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A91" s="15"/>
+      <c r="A91" s="13"/>
       <c r="B91" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C91" s="5" t="s">
         <v>51</v>
@@ -2142,9 +2134,9 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92" s="15"/>
+      <c r="A92" s="13"/>
       <c r="B92" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C92" s="5" t="s">
         <v>51</v>
@@ -2154,9 +2146,9 @@
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93" s="15"/>
+      <c r="A93" s="13"/>
       <c r="B93" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C93" s="5" t="s">
         <v>73</v>
@@ -2164,9 +2156,9 @@
       <c r="D93" s="5"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94" s="15"/>
+      <c r="A94" s="13"/>
       <c r="B94" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C94" s="6" t="s">
         <v>43</v>
@@ -2174,7 +2166,7 @@
       <c r="D94" s="5"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A95" s="15"/>
+      <c r="A95" s="13"/>
       <c r="B95" s="5" t="s">
         <v>24</v>
       </c>
@@ -2184,7 +2176,7 @@
       <c r="D95" s="5"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96" s="16"/>
+      <c r="A96" s="14"/>
       <c r="B96" s="5" t="s">
         <v>72</v>
       </c>
@@ -2193,45 +2185,45 @@
       </c>
       <c r="D96" s="5"/>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="5"/>
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="17" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C98" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A99" s="12"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="18"/>
       <c r="B99" s="5" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D99" s="5"/>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="5"/>
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A101" s="14" t="s">
-        <v>135</v>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" s="12" t="s">
+        <v>132</v>
       </c>
       <c r="B101" s="5" t="s">
         <v>39</v>
@@ -2240,11 +2232,11 @@
         <v>51</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A102" s="15"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" s="13"/>
       <c r="B102" s="5" t="s">
         <v>71</v>
       </c>
@@ -2252,67 +2244,43 @@
         <v>51</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A103" s="15"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" s="13"/>
       <c r="B103" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C103" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="F103" t="s">
-        <v>76</v>
-      </c>
-      <c r="G103">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A104" s="15"/>
+        <v>161</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" s="13"/>
       <c r="B104" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D104" s="5"/>
-      <c r="E104">
-        <v>2</v>
-      </c>
-      <c r="F104" t="s">
-        <v>77</v>
-      </c>
-      <c r="G104">
-        <v>1256</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A105" s="15"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" s="13"/>
       <c r="B105" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C105" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D105" s="5"/>
-      <c r="E105">
-        <v>3</v>
-      </c>
-      <c r="F105" t="s">
-        <v>78</v>
-      </c>
-      <c r="G105">
-        <v>7890</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A106" s="15"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" s="13"/>
       <c r="B106" s="5" t="s">
         <v>48</v>
       </c>
@@ -2321,8 +2289,8 @@
       </c>
       <c r="D106" s="5"/>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A107" s="15"/>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" s="13"/>
       <c r="B107" s="5" t="s">
         <v>50</v>
       </c>
@@ -2331,8 +2299,8 @@
       </c>
       <c r="D107" s="5"/>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A108" s="15"/>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" s="13"/>
       <c r="B108" s="5" t="s">
         <v>49</v>
       </c>
@@ -2341,8 +2309,8 @@
       </c>
       <c r="D108" s="5"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A109" s="15"/>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A109" s="13"/>
       <c r="B109" s="5" t="s">
         <v>24</v>
       </c>
@@ -2351,8 +2319,8 @@
       </c>
       <c r="D109" s="5"/>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A110" s="15"/>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A110" s="13"/>
       <c r="B110" s="5" t="s">
         <v>25</v>
       </c>
@@ -2361,20 +2329,20 @@
       </c>
       <c r="D110" s="5"/>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A111" s="15"/>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A111" s="13"/>
       <c r="B111" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C111" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D111" s="5"/>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A112" s="15"/>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A112" s="13"/>
       <c r="B112" s="5" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C112" s="5" t="s">
         <v>65</v>
@@ -2382,19 +2350,19 @@
       <c r="D112" s="5"/>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A113" s="15"/>
+      <c r="A113" s="13"/>
       <c r="B113" s="5" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D113" s="5"/>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A114" s="15"/>
+      <c r="A114" s="13"/>
       <c r="B114" s="9" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C114" s="9" t="s">
         <v>65</v>
@@ -2402,9 +2370,9 @@
       <c r="D114" s="5"/>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A115" s="15"/>
+      <c r="A115" s="13"/>
       <c r="B115" s="5" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C115" s="9" t="s">
         <v>70</v>
@@ -2412,9 +2380,9 @@
       <c r="D115" s="5"/>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A116" s="16"/>
+      <c r="A116" s="14"/>
       <c r="B116" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C116" s="9" t="s">
         <v>65</v>
@@ -2422,17 +2390,17 @@
       <c r="D116" s="5"/>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A117" s="18" t="s">
-        <v>146</v>
+      <c r="A117" s="15" t="s">
+        <v>143</v>
       </c>
       <c r="B117" s="5"/>
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A118" s="20"/>
+      <c r="A118" s="19"/>
       <c r="B118" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C118" s="9" t="s">
         <v>51</v>
@@ -2444,7 +2412,7 @@
     <row r="119" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" s="5"/>
       <c r="B119" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C119" s="9" t="s">
         <v>51</v>
@@ -2452,47 +2420,47 @@
       <c r="D119" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E119" s="13" t="s">
-        <v>149</v>
+      <c r="E119" s="21" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A120" s="14" t="s">
-        <v>137</v>
+      <c r="A120" s="12" t="s">
+        <v>134</v>
       </c>
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
       <c r="D120" s="5"/>
-      <c r="E120" s="13"/>
+      <c r="E120" s="21"/>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A121" s="15"/>
+      <c r="A121" s="13"/>
       <c r="B121" s="5" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C121" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A122" s="15"/>
+      <c r="A122" s="13"/>
       <c r="B122" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C122" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D122" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A123" s="15"/>
+      <c r="A123" s="13"/>
       <c r="B123" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C123" s="5" t="s">
         <v>51</v>
@@ -2502,7 +2470,7 @@
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A124" s="15"/>
+      <c r="A124" s="13"/>
       <c r="B124" s="5" t="s">
         <v>60</v>
       </c>
@@ -2512,9 +2480,9 @@
       <c r="D124" s="5"/>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A125" s="16"/>
+      <c r="A125" s="14"/>
       <c r="B125" s="5" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C125" s="5" t="s">
         <v>43</v>
@@ -2532,29 +2500,29 @@
       <c r="D126" s="5"/>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A127" s="14" t="s">
-        <v>138</v>
+      <c r="A127" s="12" t="s">
+        <v>135</v>
       </c>
       <c r="B127" s="5"/>
       <c r="C127" s="5"/>
       <c r="D127" s="5"/>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A128" s="15"/>
+      <c r="A128" s="13"/>
       <c r="B128" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C128" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D128" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A129" s="15"/>
+      <c r="A129" s="13"/>
       <c r="B129" s="5" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C129" s="5" t="s">
         <v>44</v>
@@ -2562,9 +2530,9 @@
       <c r="D129" s="5"/>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A130" s="15"/>
+      <c r="A130" s="13"/>
       <c r="B130" s="9" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C130" s="9" t="s">
         <v>51</v>
@@ -2574,7 +2542,7 @@
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A131" s="15"/>
+      <c r="A131" s="13"/>
       <c r="B131" s="5" t="s">
         <v>54</v>
       </c>
@@ -2584,9 +2552,9 @@
       <c r="D131" s="5"/>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A132" s="15"/>
+      <c r="A132" s="13"/>
       <c r="B132" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C132" s="5" t="s">
         <v>56</v>
@@ -2594,19 +2562,19 @@
       <c r="D132" s="5"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A133" s="15"/>
+      <c r="A133" s="13"/>
       <c r="B133" s="5" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D133" s="5"/>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A134" s="16"/>
+      <c r="A134" s="14"/>
       <c r="B134" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C134" s="5" t="s">
         <v>65</v>
@@ -2616,7 +2584,7 @@
     <row r="135" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" s="5"/>
       <c r="B135" s="5" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C135" s="5" t="s">
         <v>65</v>
@@ -2624,28 +2592,28 @@
       <c r="D135" s="5"/>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A136" s="18" t="s">
-        <v>144</v>
+      <c r="A136" s="15" t="s">
+        <v>141</v>
       </c>
       <c r="B136" s="5"/>
       <c r="C136" s="5"/>
       <c r="D136" s="5"/>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A137" s="19"/>
+      <c r="A137" s="16"/>
       <c r="B137" s="5" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C137" s="5" t="s">
         <v>51</v>
       </c>
       <c r="D137" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B138" s="5" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C138" s="5" t="s">
         <v>51</v>
@@ -2657,51 +2625,43 @@
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B139" s="8" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C139" s="8" t="s">
         <v>51</v>
       </c>
       <c r="D139" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E139" s="10"/>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A140" t="s">
-        <v>158</v>
-      </c>
-    </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141" s="22" t="s">
+        <v>155</v>
+      </c>
       <c r="B141" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C141" t="s">
         <v>43</v>
       </c>
       <c r="D141" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A142" s="22"/>
       <c r="B142" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C142" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D6" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <mergeCells count="22">
-    <mergeCell ref="A127:A134"/>
-    <mergeCell ref="A136:A137"/>
-    <mergeCell ref="A82:A87"/>
-    <mergeCell ref="A90:A96"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="A117:A118"/>
-    <mergeCell ref="A120:A125"/>
-    <mergeCell ref="A101:A116"/>
+  <mergeCells count="23">
+    <mergeCell ref="A141:A142"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="E119:E120"/>
     <mergeCell ref="E21:E22"/>
@@ -2716,6 +2676,14 @@
     <mergeCell ref="A46:A53"/>
     <mergeCell ref="A55:A62"/>
     <mergeCell ref="A64:A71"/>
+    <mergeCell ref="A127:A134"/>
+    <mergeCell ref="A136:A137"/>
+    <mergeCell ref="A82:A87"/>
+    <mergeCell ref="A90:A96"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="A120:A125"/>
+    <mergeCell ref="A101:A116"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>